<commit_message>
fixed error with spaces
</commit_message>
<xml_diff>
--- a/data/indData.xlsx
+++ b/data/indData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anders.kolstad\Documents\Github\IBECA_NINA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05DE70D-A405-4F34-A921-0A3857D61147}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03035784-AE22-4781-8D03-0456C827D4C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{FD9B3877-2BEE-49F1-96DB-153B721258FA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{FD9B3877-2BEE-49F1-96DB-153B721258FA}"/>
   </bookViews>
   <sheets>
     <sheet name="tilstandsindikatorer" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="90">
   <si>
     <t>node</t>
   </si>
@@ -305,6 +305,9 @@
   </si>
   <si>
     <t>Spurvefugler i fjellet</t>
+  </si>
+  <si>
+    <t>Ellenberg N</t>
   </si>
 </sst>
 </file>
@@ -1136,8 +1139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17FB8531-B63A-426C-9960-07BA03ABBCBC}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1333,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>37</v>
@@ -1558,7 +1561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4095CA0B-49B0-4DE4-825E-901BCBAC2241}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1643,7 +1646,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
fix problem with spaces in Ellenberg N and L
</commit_message>
<xml_diff>
--- a/data/indData.xlsx
+++ b/data/indData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anders.kolstad\Documents\Github\IBECA_NINA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03035784-AE22-4781-8D03-0456C827D4C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3799F9D-C364-4392-90C5-5FBA609AFF68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{FD9B3877-2BEE-49F1-96DB-153B721258FA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="4" xr2:uid="{FD9B3877-2BEE-49F1-96DB-153B721258FA}"/>
   </bookViews>
   <sheets>
     <sheet name="tilstandsindikatorer" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="89">
   <si>
     <t>node</t>
   </si>
@@ -70,12 +70,6 @@
     <t>NI for fjell</t>
   </si>
   <si>
-    <t>Ellenberg N</t>
-  </si>
-  <si>
-    <t>Ellenberg L</t>
-  </si>
-  <si>
     <t>Dahls R</t>
   </si>
   <si>
@@ -308,6 +302,9 @@
   </si>
   <si>
     <t>Ellenberg N</t>
+  </si>
+  <si>
+    <t>Ellenberg L</t>
   </si>
 </sst>
 </file>
@@ -546,47 +543,7 @@
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <font>
         <color theme="1"/>
@@ -1139,7 +1096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17FB8531-B63A-426C-9960-07BA03ABBCBC}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -1151,22 +1108,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1177,10 +1134,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E2" s="1">
         <v>12</v>
@@ -1195,10 +1152,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E3" s="1">
         <v>4</v>
@@ -1213,10 +1170,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E4" s="1">
         <v>13</v>
@@ -1231,10 +1188,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E5" s="1">
         <v>15</v>
@@ -1249,10 +1206,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E6" s="1">
         <v>11</v>
@@ -1267,10 +1224,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E7" s="1">
         <v>6</v>
@@ -1285,10 +1242,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E8" s="1">
         <v>4</v>
@@ -1303,10 +1260,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E9" s="1">
         <v>4</v>
@@ -1321,10 +1278,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E10" s="1">
         <v>2</v>
@@ -1336,19 +1293,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E11" s="1">
         <v>3</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1356,19 +1313,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E12" s="1">
         <v>3</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -1376,19 +1333,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E13" s="1">
         <v>3</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -1396,13 +1353,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E14" s="1">
         <v>3</v>
@@ -1414,13 +1371,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E15" s="1">
         <v>3</v>
@@ -1432,13 +1389,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E16" s="1">
         <v>10</v>
@@ -1450,13 +1407,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E17" s="1">
         <v>5</v>
@@ -1468,13 +1425,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E18" s="1">
         <v>7</v>
@@ -1486,19 +1443,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E19" s="1">
         <v>8</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -1506,19 +1463,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E20" s="1">
         <v>8</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -1526,29 +1483,29 @@
         <v>20</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C20">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
       <formula>"Påvirkning"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
       <formula>"Konsekvenser av påvirkningen"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
       <formula>"Tilstandsindikator"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
       <formula>"Påvirkningsindikator"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1574,65 +1531,65 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="5"/>
       <c r="B2" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
       <c r="B3" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
       <c r="B6" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D6" s="5"/>
     </row>
@@ -1657,19 +1614,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1677,13 +1634,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E2" s="5"/>
     </row>
@@ -1692,13 +1649,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E3" s="5"/>
     </row>
@@ -1707,13 +1664,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E4" s="5"/>
     </row>
@@ -1722,13 +1679,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E5" s="5"/>
     </row>
@@ -1737,13 +1694,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E6" s="5"/>
     </row>
@@ -1752,13 +1709,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E7" s="5"/>
     </row>
@@ -1767,13 +1724,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E8" s="5"/>
     </row>
@@ -1802,16 +1759,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -1819,7 +1776,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -1829,7 +1786,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -1839,7 +1796,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -1849,7 +1806,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -1859,7 +1816,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1869,7 +1826,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1879,10 +1836,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D8" s="5"/>
     </row>
@@ -1891,7 +1848,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1901,7 +1858,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1911,7 +1868,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -1921,7 +1878,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1931,7 +1888,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -1941,11 +1898,11 @@
         <v>13</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -1953,11 +1910,11 @@
         <v>14</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -1965,7 +1922,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -1980,8 +1937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C601D3-9EDB-4E4F-80BC-043342852ACA}">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1995,25 +1952,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -2021,7 +1978,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -2029,7 +1986,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="5"/>
       <c r="F2" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G2" s="5"/>
     </row>
@@ -2038,7 +1995,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
@@ -2046,7 +2003,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="5"/>
       <c r="F3" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G3" s="5"/>
     </row>
@@ -2055,7 +2012,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
@@ -2063,7 +2020,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="5"/>
       <c r="F4" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G4" s="5"/>
     </row>
@@ -2072,7 +2029,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
@@ -2080,7 +2037,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="5"/>
       <c r="F5" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G5" s="5"/>
     </row>
@@ -2089,7 +2046,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
@@ -2097,7 +2054,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="5"/>
       <c r="F6" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G6" s="5"/>
     </row>
@@ -2106,7 +2063,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
@@ -2114,7 +2071,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="5"/>
       <c r="F7" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G7" s="5"/>
     </row>
@@ -2123,7 +2080,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
@@ -2131,7 +2088,7 @@
       <c r="D8" s="1"/>
       <c r="E8" s="5"/>
       <c r="F8" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G8" s="5"/>
     </row>
@@ -2140,7 +2097,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>8</v>
@@ -2148,7 +2105,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="5"/>
       <c r="F9" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G9" s="5"/>
     </row>
@@ -2157,7 +2114,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>9</v>
@@ -2165,7 +2122,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="5"/>
       <c r="F10" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G10" s="5"/>
     </row>
@@ -2174,15 +2131,15 @@
         <v>10</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="5"/>
       <c r="F11" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G11" s="5"/>
     </row>
@@ -2191,15 +2148,15 @@
         <v>11</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="5"/>
       <c r="F12" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G12" s="5"/>
     </row>
@@ -2208,15 +2165,15 @@
         <v>12</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="5"/>
       <c r="F13" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G13" s="5"/>
     </row>
@@ -2225,15 +2182,15 @@
         <v>13</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="5"/>
       <c r="F14" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G14" s="5"/>
     </row>
@@ -2242,15 +2199,15 @@
         <v>14</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="5"/>
       <c r="F15" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G15" s="5"/>
     </row>
@@ -2259,15 +2216,15 @@
         <v>15</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="5"/>
       <c r="F16" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G16" s="5"/>
     </row>
@@ -2276,15 +2233,15 @@
         <v>16</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="5"/>
       <c r="F17" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G17" s="5"/>
     </row>
@@ -2293,15 +2250,15 @@
         <v>17</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="5"/>
       <c r="F18" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G18" s="5"/>
     </row>
@@ -2310,15 +2267,15 @@
         <v>18</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="5"/>
       <c r="F19" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G19" s="5"/>
     </row>
@@ -2327,15 +2284,15 @@
         <v>19</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="5"/>
       <c r="F20" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G20" s="5"/>
     </row>
@@ -2347,12 +2304,12 @@
         <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="5"/>
       <c r="F21" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G21" s="5"/>
     </row>
@@ -2364,12 +2321,12 @@
         <v>2</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="5"/>
       <c r="F22" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G22" s="5"/>
     </row>
@@ -2381,12 +2338,12 @@
         <v>3</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="5"/>
       <c r="F23" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G23" s="5"/>
     </row>
@@ -2398,12 +2355,12 @@
         <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="5"/>
       <c r="F24" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G24" s="5"/>
     </row>
@@ -2415,12 +2372,12 @@
         <v>5</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="5"/>
       <c r="F25" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G25" s="5"/>
     </row>
@@ -2432,12 +2389,12 @@
         <v>5</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="5"/>
       <c r="F26" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G26" s="5"/>
     </row>
@@ -2449,12 +2406,12 @@
         <v>6</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="5"/>
       <c r="F27" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G27" s="5"/>
     </row>
@@ -2466,12 +2423,12 @@
         <v>5</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="5"/>
       <c r="F28" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G28" s="5"/>
     </row>
@@ -2483,12 +2440,12 @@
         <v>7</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="5"/>
       <c r="F29" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G29" s="5"/>
     </row>
@@ -2500,12 +2457,12 @@
         <v>8</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="5"/>
       <c r="F30" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G30" s="5"/>
     </row>
@@ -2517,12 +2474,12 @@
         <v>9</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="5"/>
       <c r="F31" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G31" s="5"/>
     </row>
@@ -2531,15 +2488,15 @@
         <v>31</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="5"/>
       <c r="F32" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G32" s="5"/>
     </row>
@@ -2548,15 +2505,15 @@
         <v>32</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="5"/>
       <c r="F33" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G33" s="5"/>
     </row>
@@ -2565,15 +2522,15 @@
         <v>33</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="5"/>
       <c r="F34" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G34" s="5"/>
     </row>
@@ -2582,15 +2539,15 @@
         <v>34</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="5"/>
       <c r="F35" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G35" s="5"/>
     </row>
@@ -2599,15 +2556,15 @@
         <v>35</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="5"/>
       <c r="F36" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G36" s="5"/>
     </row>
@@ -2616,15 +2573,15 @@
         <v>36</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="5"/>
       <c r="F37" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G37" s="5"/>
     </row>
@@ -2633,15 +2590,15 @@
         <v>37</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="5"/>
       <c r="F38" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G38" s="5"/>
     </row>
@@ -2650,15 +2607,15 @@
         <v>38</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="5"/>
       <c r="F39" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G39" s="5"/>
     </row>
@@ -2667,15 +2624,15 @@
         <v>39</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="5"/>
       <c r="F40" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G40" s="5"/>
     </row>
@@ -2684,15 +2641,15 @@
         <v>40</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="5"/>
       <c r="F41" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G41" s="5"/>
     </row>
@@ -2701,7 +2658,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>1</v>
@@ -2709,7 +2666,7 @@
       <c r="D42" s="1"/>
       <c r="E42" s="5"/>
       <c r="F42" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G42" s="5"/>
     </row>
@@ -2718,7 +2675,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>2</v>
@@ -2726,7 +2683,7 @@
       <c r="D43" s="1"/>
       <c r="E43" s="5"/>
       <c r="F43" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G43" s="5"/>
     </row>
@@ -2735,7 +2692,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>3</v>
@@ -2743,7 +2700,7 @@
       <c r="D44" s="1"/>
       <c r="E44" s="5"/>
       <c r="F44" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G44" s="5"/>
     </row>
@@ -2752,7 +2709,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>4</v>
@@ -2760,7 +2717,7 @@
       <c r="D45" s="1"/>
       <c r="E45" s="5"/>
       <c r="F45" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G45" s="5"/>
     </row>
@@ -2769,7 +2726,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>5</v>
@@ -2777,7 +2734,7 @@
       <c r="D46" s="1"/>
       <c r="E46" s="5"/>
       <c r="F46" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G46" s="5"/>
     </row>
@@ -2786,7 +2743,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>6</v>
@@ -2794,7 +2751,7 @@
       <c r="D47" s="1"/>
       <c r="E47" s="5"/>
       <c r="F47" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G47" s="5"/>
     </row>
@@ -2803,7 +2760,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>7</v>
@@ -2811,7 +2768,7 @@
       <c r="D48" s="1"/>
       <c r="E48" s="5"/>
       <c r="F48" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G48" s="5"/>
     </row>
@@ -2820,7 +2777,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>8</v>
@@ -2828,7 +2785,7 @@
       <c r="D49" s="1"/>
       <c r="E49" s="5"/>
       <c r="F49" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G49" s="5"/>
     </row>
@@ -2837,7 +2794,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>9</v>
@@ -2845,7 +2802,7 @@
       <c r="D50" s="1"/>
       <c r="E50" s="5"/>
       <c r="F50" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G50" s="5"/>
     </row>
@@ -2854,15 +2811,15 @@
         <v>50</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="5"/>
       <c r="F51" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G51" s="5"/>
     </row>
@@ -2871,15 +2828,15 @@
         <v>51</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="5"/>
       <c r="F52" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G52" s="5"/>
     </row>
@@ -2888,15 +2845,15 @@
         <v>52</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="5"/>
       <c r="F53" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G53" s="5"/>
     </row>
@@ -2905,15 +2862,15 @@
         <v>53</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="5"/>
       <c r="F54" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G54" s="5"/>
     </row>
@@ -2922,15 +2879,15 @@
         <v>54</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="5"/>
       <c r="F55" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G55" s="5"/>
     </row>
@@ -2939,15 +2896,15 @@
         <v>55</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="5"/>
       <c r="F56" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G56" s="5"/>
     </row>
@@ -2956,15 +2913,15 @@
         <v>56</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="5"/>
       <c r="F57" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G57" s="5"/>
     </row>
@@ -2973,15 +2930,15 @@
         <v>57</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="5"/>
       <c r="F58" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G58" s="5"/>
     </row>
@@ -2990,15 +2947,15 @@
         <v>58</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="5"/>
       <c r="F59" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G59" s="5"/>
     </row>
@@ -3007,15 +2964,15 @@
         <v>59</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="5"/>
       <c r="F60" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G60" s="5"/>
     </row>
@@ -3024,7 +2981,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>1</v>
@@ -3032,7 +2989,7 @@
       <c r="D61" s="1"/>
       <c r="E61" s="5"/>
       <c r="F61" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G61" s="5"/>
     </row>
@@ -3041,7 +2998,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>2</v>
@@ -3049,7 +3006,7 @@
       <c r="D62" s="1"/>
       <c r="E62" s="5"/>
       <c r="F62" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G62" s="5"/>
     </row>
@@ -3058,7 +3015,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>3</v>
@@ -3066,7 +3023,7 @@
       <c r="D63" s="1"/>
       <c r="E63" s="5"/>
       <c r="F63" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G63" s="5"/>
     </row>
@@ -3075,7 +3032,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>5</v>
@@ -3083,7 +3040,7 @@
       <c r="D64" s="1"/>
       <c r="E64" s="5"/>
       <c r="F64" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G64" s="5"/>
     </row>
@@ -3092,7 +3049,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>6</v>
@@ -3100,7 +3057,7 @@
       <c r="D65" s="1"/>
       <c r="E65" s="5"/>
       <c r="F65" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G65" s="5"/>
     </row>
@@ -3109,7 +3066,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>7</v>
@@ -3117,7 +3074,7 @@
       <c r="D66" s="1"/>
       <c r="E66" s="5"/>
       <c r="F66" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G66" s="5"/>
     </row>
@@ -3126,7 +3083,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>9</v>
@@ -3134,7 +3091,7 @@
       <c r="D67" s="1"/>
       <c r="E67" s="5"/>
       <c r="F67" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G67" s="5"/>
     </row>
@@ -3143,15 +3100,15 @@
         <v>67</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="5"/>
       <c r="F68" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G68" s="5"/>
     </row>
@@ -3160,15 +3117,15 @@
         <v>68</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="5"/>
       <c r="F69" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G69" s="5"/>
     </row>
@@ -3177,7 +3134,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>9</v>
@@ -3185,7 +3142,7 @@
       <c r="D70" s="1"/>
       <c r="E70" s="5"/>
       <c r="F70" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G70" s="5"/>
     </row>
@@ -3194,7 +3151,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>9</v>
@@ -3202,78 +3159,78 @@
       <c r="D71" s="1"/>
       <c r="E71" s="5"/>
       <c r="F71" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G71" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B61:B69 B2:B20">
-    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
       <formula>"Påvirkning"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
       <formula>"Konsekvenser av påvirkningen"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="23" operator="equal">
       <formula>"Tilstandsindikator"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="24" operator="equal">
       <formula>"Påvirkningsindikator"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:D41">
-    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
       <formula>"Påvirkning"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
       <formula>"Konsekvenser av påvirkningen"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="19" operator="equal">
       <formula>"Tilstandsindikator"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="20" operator="equal">
       <formula>"Påvirkningsindikator"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42:B60">
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>"Påvirkning"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
       <formula>"Konsekvenser av påvirkningen"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="15" operator="equal">
       <formula>"Tilstandsindikator"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
       <formula>"Påvirkningsindikator"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B70">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"Påvirkning"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"Konsekvenser av påvirkningen"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"Tilstandsindikator"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>"Påvirkningsindikator"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B71">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Påvirkning"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Konsekvenser av påvirkningen"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Tilstandsindikator"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"Påvirkningsindikator"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>